<commit_message>
strips columns spaces in tranfers
</commit_message>
<xml_diff>
--- a/files/movimientos.xlsx
+++ b/files/movimientos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N1009"/>
+  <dimension ref="A1:M1009"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,7 +438,6 @@
     <col width="40" customWidth="1" min="11" max="11"/>
     <col width="40" customWidth="1" min="12" max="12"/>
     <col width="35" customWidth="1" min="13" max="13"/>
-    <col width="28" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -507,11 +506,6 @@
           <t>Procendecias</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Asientos</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1259,8 +1253,10 @@
       <c r="J18" t="n">
         <v>2406</v>
       </c>
-      <c r="N18" t="n">
-        <v>100057247</v>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>EMPRESA REGIONAL DE SERVICIO PUBLICO DE ELECTRICIDAD DEL NORTE S.A.</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -1303,8 +1299,10 @@
       <c r="J19" t="n">
         <v>2406</v>
       </c>
-      <c r="N19" t="n">
-        <v>100057251</v>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>EMPRESA REGIONAL DE SERVICIO PUBLICO DE ELECTRICIDAD DEL NORTE S.A.</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -1352,11 +1350,6 @@
           <t>F061 00005035 F061 000</t>
         </is>
       </c>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>EMPRESA REGIONAL DE SERVICIO PUBLICO DE ELECTRICIDAD ELECTRONOROESTE S.A.</t>
-        </is>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1398,11 +1391,6 @@
       <c r="J21" t="n">
         <v>2014</v>
       </c>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>REG LAMBAY-EDUCAC LAMBAYEQUE PPTO</t>
-        </is>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1449,11 +1437,6 @@
           <t>Referencia Beneficiari</t>
         </is>
       </c>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>WESTERN UNION PERU S.A.</t>
-        </is>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1495,11 +1478,6 @@
       <c r="J23" t="n">
         <v>2014</v>
       </c>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>HOSP JOSE H  SOTO CADENILLAS-PPTO</t>
-        </is>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1541,11 +1519,6 @@
       <c r="J24" t="n">
         <v>2014</v>
       </c>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>TRZA CONTRATISTAS Y SERVICIOS GENERALES</t>
-        </is>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1587,11 +1560,6 @@
       <c r="J25" t="n">
         <v>2014</v>
       </c>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>REGION LAMBAYEQUE-TRANSPORTES PPTO</t>
-        </is>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1633,11 +1601,6 @@
       <c r="J26" t="n">
         <v>2014</v>
       </c>
-      <c r="L26" t="inlineStr">
-        <is>
-          <t>CENTROS JUVENILES-PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1730,11 +1693,6 @@
       <c r="J28" t="n">
         <v>2014</v>
       </c>
-      <c r="L28" t="inlineStr">
-        <is>
-          <t>TRZA CONTRATISTAS Y SERVICIOS GENERALES</t>
-        </is>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1776,6 +1734,11 @@
       <c r="J29" t="n">
         <v>2401</v>
       </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>CAJA MUNICIPAL DE AHORRO Y CREDITO DE AREQUIPA</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1817,11 +1780,6 @@
       <c r="J30" t="n">
         <v>2014</v>
       </c>
-      <c r="L30" t="inlineStr">
-        <is>
-          <t>REG LAMBAY-EDUCAC LAMBAYEQUE PPTO</t>
-        </is>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1904,11 +1862,6 @@
       <c r="J32" t="n">
         <v>2014</v>
       </c>
-      <c r="L32" t="inlineStr">
-        <is>
-          <t>PROGRAMA NACIONAL DE TELECOMUNICACI</t>
-        </is>
-      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2052,11 +2005,6 @@
       <c r="J35" t="n">
         <v>2014</v>
       </c>
-      <c r="L35" t="inlineStr">
-        <is>
-          <t>MUNI DIST SANTO TOMAS PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2098,11 +2046,6 @@
       <c r="J36" t="n">
         <v>2014</v>
       </c>
-      <c r="L36" t="inlineStr">
-        <is>
-          <t>MUNI DIST SANTO TOMAS PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2348,11 +2291,6 @@
       <c r="J41" t="n">
         <v>2014</v>
       </c>
-      <c r="L41" t="inlineStr">
-        <is>
-          <t>AUTORIDAD PARA LA RECONSTRUCCION CO</t>
-        </is>
-      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -4995,11 +4933,6 @@
       <c r="J93" t="n">
         <v>2014</v>
       </c>
-      <c r="L93" t="inlineStr">
-        <is>
-          <t>MUNI DIST SANTO TOMAS PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -5500,11 +5433,6 @@
       <c r="J103" t="n">
         <v>2014</v>
       </c>
-      <c r="L103" t="inlineStr">
-        <is>
-          <t>MUNI DIST SANTO TOMAS PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -5658,9 +5586,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N106" t="n">
-        <v>7000016668</v>
-      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -6875,11 +6800,6 @@
       <c r="J130" t="n">
         <v>2014</v>
       </c>
-      <c r="L130" t="inlineStr">
-        <is>
-          <t>MIDIS SEDE CENTRAL PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -7227,11 +7147,6 @@
       <c r="J137" t="n">
         <v>2014</v>
       </c>
-      <c r="L137" t="inlineStr">
-        <is>
-          <t>MUNI DIST SANTO TOMAS PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -7426,11 +7341,6 @@
       <c r="J141" t="n">
         <v>2014</v>
       </c>
-      <c r="L141" t="inlineStr">
-        <is>
-          <t>MUNI DIST SANTO TOMAS PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -7472,11 +7382,6 @@
       <c r="J142" t="n">
         <v>2014</v>
       </c>
-      <c r="L142" t="inlineStr">
-        <is>
-          <t>MUNI DIST SANTO TOMAS PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -7518,11 +7423,6 @@
       <c r="J143" t="n">
         <v>2014</v>
       </c>
-      <c r="L143" t="inlineStr">
-        <is>
-          <t>MUNI DIST SANTO TOMAS PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -7676,9 +7576,6 @@
           <t>TRABAJADOR</t>
         </is>
       </c>
-      <c r="N146" t="n">
-        <v>7000016687</v>
-      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -8558,11 +8455,6 @@
       <c r="J165" t="n">
         <v>2014</v>
       </c>
-      <c r="L165" t="inlineStr">
-        <is>
-          <t>MUNI PROV CHICLAYO PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -8604,11 +8496,6 @@
       <c r="J166" t="n">
         <v>2014</v>
       </c>
-      <c r="L166" t="inlineStr">
-        <is>
-          <t>MUNI DIST CAYALTI PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -8650,11 +8537,6 @@
       <c r="J167" t="n">
         <v>2014</v>
       </c>
-      <c r="L167" t="inlineStr">
-        <is>
-          <t>MINDEF EP SEPTIMA BRIG INFANTERIA</t>
-        </is>
-      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -8701,11 +8583,6 @@
           <t>Referencia Beneficiari</t>
         </is>
       </c>
-      <c r="L168" t="inlineStr">
-        <is>
-          <t>WESTERN UNION PERU S.A.</t>
-        </is>
-      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -8747,9 +8624,6 @@
       <c r="J169" t="n">
         <v>2001</v>
       </c>
-      <c r="N169" t="n">
-        <v>100057131</v>
-      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -8791,11 +8665,6 @@
       <c r="J170" t="n">
         <v>2014</v>
       </c>
-      <c r="L170" t="inlineStr">
-        <is>
-          <t>MUNI DIST PIMPINGOS PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -8837,11 +8706,6 @@
       <c r="J171" t="n">
         <v>2014</v>
       </c>
-      <c r="L171" t="inlineStr">
-        <is>
-          <t>REGION CAJAMARCA-SALUD CUTERVO</t>
-        </is>
-      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -8934,6 +8798,11 @@
       <c r="J173" t="n">
         <v>2401</v>
       </c>
+      <c r="L173" t="inlineStr">
+        <is>
+          <t>CAJA MUNICIPAL DE AHORRO Y CREDITO DE AREQUIPA</t>
+        </is>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -8975,11 +8844,6 @@
       <c r="J174" t="n">
         <v>2014</v>
       </c>
-      <c r="L174" t="inlineStr">
-        <is>
-          <t>MUNI DIST YAUYUCAN PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -9072,11 +8936,6 @@
       <c r="J176" t="n">
         <v>2014</v>
       </c>
-      <c r="L176" t="inlineStr">
-        <is>
-          <t>MINDEF EP SEPTIMA BRIG INFANTERIA</t>
-        </is>
-      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -9118,11 +8977,6 @@
       <c r="J177" t="n">
         <v>2014</v>
       </c>
-      <c r="L177" t="inlineStr">
-        <is>
-          <t>MUNI DIST SAN ANDRES DE CUTERVO PRE</t>
-        </is>
-      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -9164,11 +9018,6 @@
       <c r="J178" t="n">
         <v>2014</v>
       </c>
-      <c r="L178" t="inlineStr">
-        <is>
-          <t>REG LAMBAY-EDUCAC LAMBAYEQUE PPTO</t>
-        </is>
-      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -9822,11 +9671,6 @@
       <c r="J191" t="n">
         <v>2014</v>
       </c>
-      <c r="L191" t="inlineStr">
-        <is>
-          <t>ANA - JEQUETEPEQUE-ZARUMILLA</t>
-        </is>
-      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -11194,11 +11038,6 @@
       <c r="J218" t="n">
         <v>2014</v>
       </c>
-      <c r="L218" t="inlineStr">
-        <is>
-          <t>AGRO RURAL DIREC ZONAL LAMBAYEQUE</t>
-        </is>
-      </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -11291,11 +11130,6 @@
       <c r="J220" t="n">
         <v>2014</v>
       </c>
-      <c r="L220" t="inlineStr">
-        <is>
-          <t>MUNI DIST INCAHUASI PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -11439,11 +11273,6 @@
       <c r="J223" t="n">
         <v>2014</v>
       </c>
-      <c r="L223" t="inlineStr">
-        <is>
-          <t>ANA - JEQUETEPEQUE-ZARUMILLA</t>
-        </is>
-      </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
@@ -12199,11 +12028,6 @@
       <c r="J238" t="n">
         <v>2014</v>
       </c>
-      <c r="L238" t="inlineStr">
-        <is>
-          <t>ANA - JEQUETEPEQUE-ZARUMILLA</t>
-        </is>
-      </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
@@ -12551,11 +12375,6 @@
       <c r="J245" t="n">
         <v>2014</v>
       </c>
-      <c r="L245" t="inlineStr">
-        <is>
-          <t>DIR EJEC INVESTIG CRIMINAL Y APOYO</t>
-        </is>
-      </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
@@ -13362,11 +13181,6 @@
       <c r="J261" t="n">
         <v>2014</v>
       </c>
-      <c r="L261" t="inlineStr">
-        <is>
-          <t>MINDEF EP SEPTIMA BRIG INFANTERIA</t>
-        </is>
-      </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
@@ -13459,11 +13273,6 @@
       <c r="J263" t="n">
         <v>2014</v>
       </c>
-      <c r="L263" t="inlineStr">
-        <is>
-          <t>ORG SUP INVERSION ENERGIA Y MINERIA</t>
-        </is>
-      </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
@@ -13556,11 +13365,6 @@
       <c r="J265" t="n">
         <v>2014</v>
       </c>
-      <c r="L265" t="inlineStr">
-        <is>
-          <t>AGRO RURAL DIREC ZONAL LAMBAYEQUE</t>
-        </is>
-      </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
@@ -14010,9 +13814,6 @@
       <c r="J274" t="n">
         <v>2001</v>
       </c>
-      <c r="N274" t="n">
-        <v>100057133</v>
-      </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
@@ -14207,11 +14008,6 @@
       <c r="J278" t="n">
         <v>2014</v>
       </c>
-      <c r="L278" t="inlineStr">
-        <is>
-          <t>AGRO RURAL DIREC ZONAL LAMBAYEQUE</t>
-        </is>
-      </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
@@ -14309,11 +14105,6 @@
           <t>0000010041</t>
         </is>
       </c>
-      <c r="L280" t="inlineStr">
-        <is>
-          <t>TERMOSELVA S.R.L.</t>
-        </is>
-      </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
@@ -14360,11 +14151,6 @@
           <t>Referencia Beneficiari</t>
         </is>
       </c>
-      <c r="L281" t="inlineStr">
-        <is>
-          <t>FIDEICOMISO TRES HERMANAS</t>
-        </is>
-      </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
@@ -14411,11 +14197,6 @@
           <t>Referencia Beneficiari</t>
         </is>
       </c>
-      <c r="L282" t="inlineStr">
-        <is>
-          <t>FIDEICOMISO MARCONA</t>
-        </is>
-      </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
@@ -15383,8 +15164,10 @@
       <c r="J304" t="n">
         <v>2406</v>
       </c>
-      <c r="N304" t="n">
-        <v>100057062</v>
+      <c r="L304" t="inlineStr">
+        <is>
+          <t>EMPRESA REGIONAL DE SERVICIO PUBLICO DE ELECTRICIDAD DEL NORTE S.A.</t>
+        </is>
       </c>
     </row>
     <row r="305">
@@ -15427,6 +15210,11 @@
       <c r="J305" t="n">
         <v>2401</v>
       </c>
+      <c r="L305" t="inlineStr">
+        <is>
+          <t>AGRO PIMA PERU SAC</t>
+        </is>
+      </c>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
@@ -15473,14 +15261,6 @@
           <t>Referencia Beneficiari</t>
         </is>
       </c>
-      <c r="L306" t="inlineStr">
-        <is>
-          <t>WESTERN UNION PERU S.A.</t>
-        </is>
-      </c>
-      <c r="N306" t="n">
-        <v>7000016649</v>
-      </c>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
@@ -15522,11 +15302,6 @@
       <c r="J307" t="n">
         <v>2014</v>
       </c>
-      <c r="L307" t="inlineStr">
-        <is>
-          <t>ATC SITIOS DEL PERU  SCRL</t>
-        </is>
-      </c>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
@@ -15568,8 +15343,10 @@
       <c r="J308" t="n">
         <v>2401</v>
       </c>
-      <c r="N308" t="n">
-        <v>7000016645</v>
+      <c r="L308" t="inlineStr">
+        <is>
+          <t>CAJA MUNICIPAL DE AHORRO Y CREDITO DE AREQUIPA</t>
+        </is>
       </c>
     </row>
     <row r="309">
@@ -16795,9 +16572,6 @@
           <t>TRABAJADOR</t>
         </is>
       </c>
-      <c r="N332" t="n">
-        <v>100057097</v>
-      </c>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
@@ -17104,9 +16878,6 @@
           <t>TRABAJADOR</t>
         </is>
       </c>
-      <c r="N338" t="n">
-        <v>100057235</v>
-      </c>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
@@ -19280,9 +19051,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N381" t="n">
-        <v>7000016686</v>
-      </c>
     </row>
     <row r="382">
       <c r="A382" t="inlineStr">
@@ -22897,9 +22665,6 @@
       <c r="J460" t="n">
         <v>2505</v>
       </c>
-      <c r="N460" t="n">
-        <v>100033222</v>
-      </c>
     </row>
     <row r="461">
       <c r="A461" t="inlineStr">
@@ -22941,8 +22706,10 @@
       <c r="J461" t="n">
         <v>2406</v>
       </c>
-      <c r="N461" t="n">
-        <v>100033219</v>
+      <c r="L461" t="inlineStr">
+        <is>
+          <t>EMPRESA REGIONAL DE SERVICIO PUBLICO DE ELECTRICIDAD DEL NORTE S.A.</t>
+        </is>
       </c>
     </row>
     <row r="462">
@@ -22990,11 +22757,6 @@
           <t>PAGO PROVEEDORES RIPLE</t>
         </is>
       </c>
-      <c r="L462" t="inlineStr">
-        <is>
-          <t>MALL AVENTURA S.A.</t>
-        </is>
-      </c>
     </row>
     <row r="463">
       <c r="A463" t="inlineStr">
@@ -23041,14 +22803,6 @@
           <t>Referencia Beneficiari</t>
         </is>
       </c>
-      <c r="L463" t="inlineStr">
-        <is>
-          <t>WESTERN UNION PERU S.A.</t>
-        </is>
-      </c>
-      <c r="N463" t="n">
-        <v>7000016627</v>
-      </c>
     </row>
     <row r="464">
       <c r="A464" t="inlineStr">
@@ -23095,14 +22849,6 @@
           <t>Referencia Beneficiari</t>
         </is>
       </c>
-      <c r="L464" t="inlineStr">
-        <is>
-          <t>GTD PERU S.A</t>
-        </is>
-      </c>
-      <c r="N464" t="n">
-        <v>6500005053</v>
-      </c>
     </row>
     <row r="465">
       <c r="A465" t="inlineStr">
@@ -23144,14 +22890,6 @@
       <c r="J465" t="n">
         <v>2014</v>
       </c>
-      <c r="L465" t="inlineStr">
-        <is>
-          <t>REG CAJAMARCA EDUCAC CHOTA PPTO</t>
-        </is>
-      </c>
-      <c r="N465" t="n">
-        <v>7000016670</v>
-      </c>
     </row>
     <row r="466">
       <c r="A466" t="inlineStr">
@@ -23193,6 +22931,11 @@
       <c r="J466" t="n">
         <v>2401</v>
       </c>
+      <c r="L466" t="inlineStr">
+        <is>
+          <t>CABLENORTV SAC</t>
+        </is>
+      </c>
     </row>
     <row r="467">
       <c r="A467" t="inlineStr">
@@ -23285,11 +23028,6 @@
       <c r="J468" t="n">
         <v>2014</v>
       </c>
-      <c r="L468" t="inlineStr">
-        <is>
-          <t>MUNI DIST PIMENTEL PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="469">
       <c r="A469" t="inlineStr">
@@ -23331,11 +23069,6 @@
       <c r="J469" t="n">
         <v>2014</v>
       </c>
-      <c r="L469" t="inlineStr">
-        <is>
-          <t>INABIF PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="470">
       <c r="A470" t="inlineStr">
@@ -23734,8 +23467,10 @@
       <c r="J477" t="n">
         <v>2401</v>
       </c>
-      <c r="N477" t="n">
-        <v>7000016622</v>
+      <c r="L477" t="inlineStr">
+        <is>
+          <t>CAJA MUNICIPAL DE AHORRO Y CREDITO DE AREQUIPA</t>
+        </is>
       </c>
     </row>
     <row r="478">
@@ -23778,11 +23513,6 @@
       <c r="J478" t="n">
         <v>2014</v>
       </c>
-      <c r="L478" t="inlineStr">
-        <is>
-          <t>SUPER NAC SERVICIOS DE SANEAMIENTO</t>
-        </is>
-      </c>
     </row>
     <row r="479">
       <c r="A479" t="inlineStr">
@@ -23987,9 +23717,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N482" t="n">
-        <v>7000016684</v>
-      </c>
     </row>
     <row r="483">
       <c r="A483" t="inlineStr">
@@ -24551,9 +24278,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N493" t="n">
-        <v>7000016682</v>
-      </c>
     </row>
     <row r="494">
       <c r="A494" t="inlineStr">
@@ -25319,9 +25043,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N508" t="n">
-        <v>7000016685</v>
-      </c>
     </row>
     <row r="509">
       <c r="A509" t="inlineStr">
@@ -25628,9 +25349,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N514" t="n">
-        <v>7000016681</v>
-      </c>
     </row>
     <row r="515">
       <c r="A515" t="inlineStr">
@@ -26651,9 +26369,6 @@
           <t>TRABAJADOR</t>
         </is>
       </c>
-      <c r="N534" t="n">
-        <v>100057096</v>
-      </c>
     </row>
     <row r="535">
       <c r="A535" t="inlineStr">
@@ -26756,9 +26471,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N536" t="n">
-        <v>7000016683</v>
-      </c>
     </row>
     <row r="537">
       <c r="A537" t="inlineStr">
@@ -26907,14 +26619,6 @@
           <t>0000010041</t>
         </is>
       </c>
-      <c r="L539" t="inlineStr">
-        <is>
-          <t>KALLPA GENERACION SA</t>
-        </is>
-      </c>
-      <c r="N539" t="n">
-        <v>6500005051</v>
-      </c>
     </row>
     <row r="540">
       <c r="A540" t="inlineStr">
@@ -27165,14 +26869,6 @@
           <t>0000010041</t>
         </is>
       </c>
-      <c r="L544" t="inlineStr">
-        <is>
-          <t>ORAZUL ENERGY PERU SA</t>
-        </is>
-      </c>
-      <c r="N544" t="n">
-        <v>6500005052</v>
-      </c>
     </row>
     <row r="545">
       <c r="A545" t="inlineStr">
@@ -27265,6 +26961,11 @@
       <c r="J546" t="n">
         <v>2401</v>
       </c>
+      <c r="L546" t="inlineStr">
+        <is>
+          <t>EMPRESA DE GENERACION ELECTRICA MACHUPICCHU S.A.</t>
+        </is>
+      </c>
     </row>
     <row r="547">
       <c r="A547" t="inlineStr">
@@ -28293,9 +27994,6 @@
       <c r="J569" t="n">
         <v>2505</v>
       </c>
-      <c r="N569" t="n">
-        <v>100032879</v>
-      </c>
     </row>
     <row r="570">
       <c r="A570" t="inlineStr">
@@ -28337,8 +28035,10 @@
       <c r="J570" t="n">
         <v>2406</v>
       </c>
-      <c r="N570" t="n">
-        <v>100032893</v>
+      <c r="L570" t="inlineStr">
+        <is>
+          <t>EMPRESA REGIONAL DE SERVICIO PUBLICO DE ELECTRICIDAD DEL NORTE S.A.</t>
+        </is>
       </c>
     </row>
     <row r="571">
@@ -28427,14 +28127,6 @@
           <t>ELECTROCENTRO S.A.</t>
         </is>
       </c>
-      <c r="L572" t="inlineStr">
-        <is>
-          <t>ELECTROCENTRO S.A</t>
-        </is>
-      </c>
-      <c r="N572" t="n">
-        <v>6500005054</v>
-      </c>
     </row>
     <row r="573">
       <c r="A573" t="inlineStr">
@@ -28476,11 +28168,6 @@
       <c r="J573" t="n">
         <v>2014</v>
       </c>
-      <c r="L573" t="inlineStr">
-        <is>
-          <t>MUNI DIST PATAPO PPTO</t>
-        </is>
-      </c>
     </row>
     <row r="574">
       <c r="A574" t="inlineStr">
@@ -28522,11 +28209,6 @@
       <c r="J574" t="n">
         <v>2014</v>
       </c>
-      <c r="L574" t="inlineStr">
-        <is>
-          <t>MUNI DIST PATAPO PPTO</t>
-        </is>
-      </c>
     </row>
     <row r="575">
       <c r="A575" t="inlineStr">
@@ -28568,11 +28250,6 @@
       <c r="J575" t="n">
         <v>2401</v>
       </c>
-      <c r="L575" t="inlineStr">
-        <is>
-          <t>EMPRESA REGIONAL DE SERVICIO PUBLICO DE ELECTRICIDAD ELECTRONORTE MEDIO S.A</t>
-        </is>
-      </c>
     </row>
     <row r="576">
       <c r="A576" t="inlineStr">
@@ -28614,11 +28291,6 @@
       <c r="J576" t="n">
         <v>2014</v>
       </c>
-      <c r="L576" t="inlineStr">
-        <is>
-          <t>MUNI DIST JOSE L ORTIZ PPTO</t>
-        </is>
-      </c>
     </row>
     <row r="577">
       <c r="A577" t="inlineStr">
@@ -28706,14 +28378,6 @@
           <t>Referencia Beneficiari</t>
         </is>
       </c>
-      <c r="L578" t="inlineStr">
-        <is>
-          <t>WESTERN UNION PERU S.A.</t>
-        </is>
-      </c>
-      <c r="N578" t="n">
-        <v>7000016441</v>
-      </c>
     </row>
     <row r="579">
       <c r="A579" t="inlineStr">
@@ -28806,11 +28470,6 @@
       <c r="J580" t="n">
         <v>2014</v>
       </c>
-      <c r="L580" t="inlineStr">
-        <is>
-          <t>REGION CAJAMARCA-SALUD CUTERVO</t>
-        </is>
-      </c>
     </row>
     <row r="581">
       <c r="A581" t="inlineStr">
@@ -28852,11 +28511,6 @@
       <c r="J581" t="n">
         <v>2014</v>
       </c>
-      <c r="L581" t="inlineStr">
-        <is>
-          <t>MUNI DIST JOSE L ORTIZ PPTO</t>
-        </is>
-      </c>
     </row>
     <row r="582">
       <c r="A582" t="inlineStr">
@@ -28898,11 +28552,6 @@
       <c r="J582" t="n">
         <v>2014</v>
       </c>
-      <c r="L582" t="inlineStr">
-        <is>
-          <t>IRTP PPTO 2003</t>
-        </is>
-      </c>
     </row>
     <row r="583">
       <c r="A583" t="inlineStr">
@@ -28944,6 +28593,11 @@
       <c r="J583" t="n">
         <v>2401</v>
       </c>
+      <c r="L583" t="inlineStr">
+        <is>
+          <t>AI INVERSIONES PALO ALTO II SAC</t>
+        </is>
+      </c>
     </row>
     <row r="584">
       <c r="A584" t="inlineStr">
@@ -29036,8 +28690,10 @@
       <c r="J585" t="n">
         <v>2401</v>
       </c>
-      <c r="N585" t="n">
-        <v>6500005079</v>
+      <c r="L585" t="inlineStr">
+        <is>
+          <t>CABLENORTV SAC</t>
+        </is>
       </c>
     </row>
     <row r="586">
@@ -29080,11 +28736,6 @@
       <c r="J586" t="n">
         <v>2014</v>
       </c>
-      <c r="L586" t="inlineStr">
-        <is>
-          <t>MUNI DIST MONSEFU PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="587">
       <c r="A587" t="inlineStr">
@@ -29187,9 +28838,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N588" t="n">
-        <v>7000016466</v>
-      </c>
     </row>
     <row r="589">
       <c r="A589" t="inlineStr">
@@ -29241,9 +28889,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N589" t="n">
-        <v>7000016478</v>
-      </c>
     </row>
     <row r="590">
       <c r="A590" t="inlineStr">
@@ -29346,9 +28991,6 @@
           <t>TRABAJADOR</t>
         </is>
       </c>
-      <c r="N591" t="n">
-        <v>100032751</v>
-      </c>
     </row>
     <row r="592">
       <c r="A592" t="inlineStr">
@@ -29390,8 +29032,10 @@
       <c r="J592" t="n">
         <v>2401</v>
       </c>
-      <c r="N592" t="n">
-        <v>7000016438</v>
+      <c r="L592" t="inlineStr">
+        <is>
+          <t>CAJA MUNICIPAL DE AHORRO Y CREDITO DE AREQUIPA</t>
+        </is>
       </c>
     </row>
     <row r="593">
@@ -29495,9 +29139,6 @@
           <t>TRABAJADOR</t>
         </is>
       </c>
-      <c r="N594" t="n">
-        <v>100057052</v>
-      </c>
     </row>
     <row r="595">
       <c r="A595" t="inlineStr">
@@ -29600,9 +29241,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N596" t="n">
-        <v>7000016575</v>
-      </c>
     </row>
     <row r="597">
       <c r="A597" t="inlineStr">
@@ -29654,9 +29292,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N597" t="n">
-        <v>7000016574</v>
-      </c>
     </row>
     <row r="598">
       <c r="A598" t="inlineStr">
@@ -29861,9 +29496,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N601" t="n">
-        <v>7000016584</v>
-      </c>
     </row>
     <row r="602">
       <c r="A602" t="inlineStr">
@@ -29915,9 +29547,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N602" t="n">
-        <v>7000016578</v>
-      </c>
     </row>
     <row r="603">
       <c r="A603" t="inlineStr">
@@ -29969,9 +29598,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N603" t="n">
-        <v>7000016473</v>
-      </c>
     </row>
     <row r="604">
       <c r="A604" t="inlineStr">
@@ -30023,9 +29649,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N604" t="n">
-        <v>7000016572</v>
-      </c>
     </row>
     <row r="605">
       <c r="A605" t="inlineStr">
@@ -30128,9 +29751,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N606" t="n">
-        <v>7000016462</v>
-      </c>
     </row>
     <row r="607">
       <c r="A607" t="inlineStr">
@@ -30233,9 +29853,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N608" t="n">
-        <v>7000016582</v>
-      </c>
     </row>
     <row r="609">
       <c r="A609" t="inlineStr">
@@ -30338,9 +29955,6 @@
           <t>TRABAJADOR</t>
         </is>
       </c>
-      <c r="N610" t="n">
-        <v>100057095</v>
-      </c>
     </row>
     <row r="611">
       <c r="A611" t="inlineStr">
@@ -30392,9 +30006,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N611" t="n">
-        <v>7000016474</v>
-      </c>
     </row>
     <row r="612">
       <c r="A612" t="inlineStr">
@@ -30446,9 +30057,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N612" t="n">
-        <v>7000016592</v>
-      </c>
     </row>
     <row r="613">
       <c r="A613" t="inlineStr">
@@ -30806,9 +30414,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N619" t="n">
-        <v>7000016571</v>
-      </c>
     </row>
     <row r="620">
       <c r="A620" t="inlineStr">
@@ -31115,9 +30720,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N625" t="n">
-        <v>7000016465</v>
-      </c>
     </row>
     <row r="626">
       <c r="A626" t="inlineStr">
@@ -31169,9 +30771,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N626" t="n">
-        <v>7000016458</v>
-      </c>
     </row>
     <row r="627">
       <c r="A627" t="inlineStr">
@@ -31223,9 +30822,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N627" t="n">
-        <v>7000016472</v>
-      </c>
     </row>
     <row r="628">
       <c r="A628" t="inlineStr">
@@ -31277,9 +30873,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N628" t="n">
-        <v>7000016463</v>
-      </c>
     </row>
     <row r="629">
       <c r="A629" t="inlineStr">
@@ -31331,9 +30924,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N629" t="n">
-        <v>7000016479</v>
-      </c>
     </row>
     <row r="630">
       <c r="A630" t="inlineStr">
@@ -31385,9 +30975,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N630" t="n">
-        <v>7000016590</v>
-      </c>
     </row>
     <row r="631">
       <c r="A631" t="inlineStr">
@@ -31643,9 +31230,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N635" t="n">
-        <v>7000016481</v>
-      </c>
     </row>
     <row r="636">
       <c r="A636" t="inlineStr">
@@ -31697,9 +31281,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N636" t="n">
-        <v>7000016476</v>
-      </c>
     </row>
     <row r="637">
       <c r="A637" t="inlineStr">
@@ -31751,9 +31332,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N637" t="n">
-        <v>7000016586</v>
-      </c>
     </row>
     <row r="638">
       <c r="A638" t="inlineStr">
@@ -31805,9 +31383,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N638" t="n">
-        <v>7000016477</v>
-      </c>
     </row>
     <row r="639">
       <c r="A639" t="inlineStr">
@@ -31859,9 +31434,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N639" t="n">
-        <v>7000016587</v>
-      </c>
     </row>
     <row r="640">
       <c r="A640" t="inlineStr">
@@ -31913,9 +31485,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N640" t="n">
-        <v>7000016577</v>
-      </c>
     </row>
     <row r="641">
       <c r="A641" t="inlineStr">
@@ -31967,9 +31536,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N641" t="n">
-        <v>7000016471</v>
-      </c>
     </row>
     <row r="642">
       <c r="A642" t="inlineStr">
@@ -32021,9 +31587,6 @@
           <t>TRABAJADOR</t>
         </is>
       </c>
-      <c r="N642" t="n">
-        <v>100032751</v>
-      </c>
     </row>
     <row r="643">
       <c r="A643" t="inlineStr">
@@ -32075,9 +31638,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N643" t="n">
-        <v>7000016470</v>
-      </c>
     </row>
     <row r="644">
       <c r="A644" t="inlineStr">
@@ -32476,9 +32036,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N651" t="n">
-        <v>7000016454</v>
-      </c>
     </row>
     <row r="652">
       <c r="A652" t="inlineStr">
@@ -32632,9 +32189,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N654" t="n">
-        <v>7000016579</v>
-      </c>
     </row>
     <row r="655">
       <c r="A655" t="inlineStr">
@@ -32686,9 +32240,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N655" t="n">
-        <v>7000016581</v>
-      </c>
     </row>
     <row r="656">
       <c r="A656" t="inlineStr">
@@ -32791,9 +32342,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N657" t="n">
-        <v>7000016580</v>
-      </c>
     </row>
     <row r="658">
       <c r="A658" t="inlineStr">
@@ -33090,11 +32638,6 @@
       <c r="J663" t="n">
         <v>2014</v>
       </c>
-      <c r="L663" t="inlineStr">
-        <is>
-          <t>II DIR TERRITORIAL POLICIA CHICLAYO</t>
-        </is>
-      </c>
     </row>
     <row r="664">
       <c r="A664" t="inlineStr">
@@ -33136,11 +32679,6 @@
       <c r="J664" t="n">
         <v>2014</v>
       </c>
-      <c r="L664" t="inlineStr">
-        <is>
-          <t>MUNI DIST MONSEFU PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="665">
       <c r="A665" t="inlineStr">
@@ -33192,9 +32730,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N665" t="n">
-        <v>7000016468</v>
-      </c>
     </row>
     <row r="666">
       <c r="A666" t="inlineStr">
@@ -33348,9 +32883,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N668" t="n">
-        <v>7000016591</v>
-      </c>
     </row>
     <row r="669">
       <c r="A669" t="inlineStr">
@@ -33402,9 +32934,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N669" t="n">
-        <v>7000016459</v>
-      </c>
     </row>
     <row r="670">
       <c r="A670" t="inlineStr">
@@ -33456,9 +32985,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N670" t="n">
-        <v>7000016461</v>
-      </c>
     </row>
     <row r="671">
       <c r="A671" t="inlineStr">
@@ -33510,9 +33036,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N671" t="n">
-        <v>7000016482</v>
-      </c>
     </row>
     <row r="672">
       <c r="A672" t="inlineStr">
@@ -33564,9 +33087,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N672" t="n">
-        <v>7000016460</v>
-      </c>
     </row>
     <row r="673">
       <c r="A673" t="inlineStr">
@@ -33669,9 +33189,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N674" t="n">
-        <v>7000016588</v>
-      </c>
     </row>
     <row r="675">
       <c r="A675" t="inlineStr">
@@ -33825,9 +33342,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N677" t="n">
-        <v>7000016457</v>
-      </c>
     </row>
     <row r="678">
       <c r="A678" t="inlineStr">
@@ -33879,9 +33393,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N678" t="n">
-        <v>7000016483</v>
-      </c>
     </row>
     <row r="679">
       <c r="A679" t="inlineStr">
@@ -33933,9 +33444,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N679" t="n">
-        <v>7000016464</v>
-      </c>
     </row>
     <row r="680">
       <c r="A680" t="inlineStr">
@@ -33987,9 +33495,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N680" t="n">
-        <v>7000016456</v>
-      </c>
     </row>
     <row r="681">
       <c r="A681" t="inlineStr">
@@ -34041,9 +33546,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N681" t="n">
-        <v>7000016455</v>
-      </c>
     </row>
     <row r="682">
       <c r="A682" t="inlineStr">
@@ -34095,9 +33597,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N682" t="n">
-        <v>7000016480</v>
-      </c>
     </row>
     <row r="683">
       <c r="A683" t="inlineStr">
@@ -34149,9 +33648,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N683" t="n">
-        <v>7000016475</v>
-      </c>
     </row>
     <row r="684">
       <c r="A684" t="inlineStr">
@@ -34203,9 +33699,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N684" t="n">
-        <v>7000016469</v>
-      </c>
     </row>
     <row r="685">
       <c r="A685" t="inlineStr">
@@ -34257,9 +33750,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N685" t="n">
-        <v>7000016589</v>
-      </c>
     </row>
     <row r="686">
       <c r="A686" t="inlineStr">
@@ -34362,9 +33852,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N687" t="n">
-        <v>7000016573</v>
-      </c>
     </row>
     <row r="688">
       <c r="A688" t="inlineStr">
@@ -34416,9 +33903,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N688" t="n">
-        <v>7000016467</v>
-      </c>
     </row>
     <row r="689">
       <c r="A689" t="inlineStr">
@@ -34664,11 +34148,6 @@
       <c r="J693" t="n">
         <v>2014</v>
       </c>
-      <c r="L693" t="inlineStr">
-        <is>
-          <t>MUNI DIST MONSEFU PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="694">
       <c r="A694" t="inlineStr">
@@ -34812,11 +34291,6 @@
       <c r="J696" t="n">
         <v>2014</v>
       </c>
-      <c r="L696" t="inlineStr">
-        <is>
-          <t>MUNI DIST MONSEFU PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="697">
       <c r="A697" t="inlineStr">
@@ -34914,14 +34388,6 @@
           <t>DocSAP 2000005494 Ao 2</t>
         </is>
       </c>
-      <c r="L698" t="inlineStr">
-        <is>
-          <t>ENGIE ENERGIA PERU S.A.</t>
-        </is>
-      </c>
-      <c r="N698" t="n">
-        <v>6500005049</v>
-      </c>
     </row>
     <row r="699">
       <c r="A699" t="inlineStr">
@@ -35014,14 +34480,6 @@
       <c r="J700" t="n">
         <v>2401</v>
       </c>
-      <c r="L700" t="inlineStr">
-        <is>
-          <t>EMPRESA DE GENERACION ELECTRICA DE AREQUIPA S.A.</t>
-        </is>
-      </c>
-      <c r="N700" t="n">
-        <v>6500005050</v>
-      </c>
     </row>
     <row r="701">
       <c r="A701" t="inlineStr">
@@ -35063,14 +34521,6 @@
       <c r="J701" t="n">
         <v>2401</v>
       </c>
-      <c r="L701" t="inlineStr">
-        <is>
-          <t>INLAND ENERGY SAC</t>
-        </is>
-      </c>
-      <c r="N701" t="n">
-        <v>6500005048</v>
-      </c>
     </row>
     <row r="702">
       <c r="A702" t="inlineStr">
@@ -35112,11 +34562,6 @@
       <c r="J702" t="n">
         <v>2014</v>
       </c>
-      <c r="L702" t="inlineStr">
-        <is>
-          <t>HIDROELECTRICA HUANCHOR S A C</t>
-        </is>
-      </c>
     </row>
     <row r="703">
       <c r="A703" t="inlineStr">
@@ -35158,11 +34603,6 @@
       <c r="J703" t="n">
         <v>2014</v>
       </c>
-      <c r="L703" t="inlineStr">
-        <is>
-          <t>EMPRESA DE GENERACION ELECTRICA RIO BA OS SA</t>
-        </is>
-      </c>
     </row>
     <row r="704">
       <c r="A704" t="inlineStr">
@@ -35598,9 +35038,6 @@
       <c r="J713" t="n">
         <v>2505</v>
       </c>
-      <c r="N713" t="n">
-        <v>100032727</v>
-      </c>
     </row>
     <row r="714">
       <c r="A714" t="inlineStr">
@@ -35642,8 +35079,10 @@
       <c r="J714" t="n">
         <v>2406</v>
       </c>
-      <c r="N714" t="n">
-        <v>100032721</v>
+      <c r="L714" t="inlineStr">
+        <is>
+          <t>EMPRESA REGIONAL DE SERVICIO PUBLICO DE ELECTRICIDAD DEL NORTE S.A.</t>
+        </is>
       </c>
     </row>
     <row r="715">
@@ -35686,8 +35125,10 @@
       <c r="J715" t="n">
         <v>2406</v>
       </c>
-      <c r="N715" t="n">
-        <v>100032719</v>
+      <c r="L715" t="inlineStr">
+        <is>
+          <t>EMPRESA REGIONAL DE SERVICIO PUBLICO DE ELECTRICIDAD DEL NORTE S.A.</t>
+        </is>
       </c>
     </row>
     <row r="716">
@@ -35730,11 +35171,6 @@
       <c r="J716" t="n">
         <v>2014</v>
       </c>
-      <c r="L716" t="inlineStr">
-        <is>
-          <t>GOB LAMBAY-HOSP DOC LAS MERCED PPTO</t>
-        </is>
-      </c>
     </row>
     <row r="717">
       <c r="A717" t="inlineStr">
@@ -35781,14 +35217,6 @@
           <t>Referencia Beneficiari</t>
         </is>
       </c>
-      <c r="L717" t="inlineStr">
-        <is>
-          <t>VIETTEL PERU S.A.C.</t>
-        </is>
-      </c>
-      <c r="N717" t="n">
-        <v>6500005077</v>
-      </c>
     </row>
     <row r="718">
       <c r="A718" t="inlineStr">
@@ -35830,14 +35258,6 @@
       <c r="J718" t="n">
         <v>2014</v>
       </c>
-      <c r="L718" t="inlineStr">
-        <is>
-          <t>GERENCIA REGIONAL DE EDUCACION LAMB</t>
-        </is>
-      </c>
-      <c r="N718" t="n">
-        <v>7000016316</v>
-      </c>
     </row>
     <row r="719">
       <c r="A719" t="inlineStr">
@@ -35879,6 +35299,11 @@
       <c r="J719" t="n">
         <v>2401</v>
       </c>
+      <c r="L719" t="inlineStr">
+        <is>
+          <t>EMPRESA DE GENERACION ELECTRICA MACHUPICCHU S.A.</t>
+        </is>
+      </c>
     </row>
     <row r="720">
       <c r="A720" t="inlineStr">
@@ -35920,8 +35345,10 @@
       <c r="J720" t="n">
         <v>2401</v>
       </c>
-      <c r="N720" t="n">
-        <v>7000016323</v>
+      <c r="L720" t="inlineStr">
+        <is>
+          <t>DANPER TRUJILLO S.A.C.</t>
+        </is>
       </c>
     </row>
     <row r="721">
@@ -35964,11 +35391,6 @@
       <c r="J721" t="n">
         <v>2014</v>
       </c>
-      <c r="L721" t="inlineStr">
-        <is>
-          <t>MUNI PROV SANTA CRUZ</t>
-        </is>
-      </c>
     </row>
     <row r="722">
       <c r="A722" t="inlineStr">
@@ -36051,14 +35473,6 @@
       <c r="J723" t="n">
         <v>2014</v>
       </c>
-      <c r="L723" t="inlineStr">
-        <is>
-          <t>GERENCIA REGIONAL DE EDUCACION LAMB</t>
-        </is>
-      </c>
-      <c r="N723" t="n">
-        <v>7000016314</v>
-      </c>
     </row>
     <row r="724">
       <c r="A724" t="inlineStr">
@@ -36100,11 +35514,6 @@
       <c r="J724" t="n">
         <v>2014</v>
       </c>
-      <c r="L724" t="inlineStr">
-        <is>
-          <t>MUNI DIST MANUEL A MESONES MURO PPT</t>
-        </is>
-      </c>
     </row>
     <row r="725">
       <c r="A725" t="inlineStr">
@@ -36146,11 +35555,6 @@
       <c r="J725" t="n">
         <v>2014</v>
       </c>
-      <c r="L725" t="inlineStr">
-        <is>
-          <t>IPD PPTO 2003</t>
-        </is>
-      </c>
     </row>
     <row r="726">
       <c r="A726" t="inlineStr">
@@ -36192,11 +35596,6 @@
       <c r="J726" t="n">
         <v>2014</v>
       </c>
-      <c r="L726" t="inlineStr">
-        <is>
-          <t>MUNI DIST MANUEL A MESONES MURO PPT</t>
-        </is>
-      </c>
     </row>
     <row r="727">
       <c r="A727" t="inlineStr">
@@ -36243,14 +35642,6 @@
           <t>Referencia Beneficiari</t>
         </is>
       </c>
-      <c r="L727" t="inlineStr">
-        <is>
-          <t>WESTERN UNION PERU S.A.</t>
-        </is>
-      </c>
-      <c r="N727" t="n">
-        <v>7000016271</v>
-      </c>
     </row>
     <row r="728">
       <c r="A728" t="inlineStr">
@@ -36292,11 +35683,6 @@
       <c r="J728" t="n">
         <v>2014</v>
       </c>
-      <c r="L728" t="inlineStr">
-        <is>
-          <t>MUNI DIST MANUEL A MESONES MURO PPT</t>
-        </is>
-      </c>
     </row>
     <row r="729">
       <c r="A729" t="inlineStr">
@@ -36338,8 +35724,10 @@
       <c r="J729" t="n">
         <v>2401</v>
       </c>
-      <c r="N729" t="n">
-        <v>7000016269</v>
+      <c r="L729" t="inlineStr">
+        <is>
+          <t>CAJA MUNICIPAL DE AHORRO Y CREDITO DE AREQUIPA</t>
+        </is>
       </c>
     </row>
     <row r="730">
@@ -36382,14 +35770,6 @@
       <c r="J730" t="n">
         <v>2014</v>
       </c>
-      <c r="L730" t="inlineStr">
-        <is>
-          <t>GERENCIA REGIONAL DE EDUCACION LAMB</t>
-        </is>
-      </c>
-      <c r="N730" t="n">
-        <v>7000016315</v>
-      </c>
     </row>
     <row r="731">
       <c r="A731" t="inlineStr">
@@ -36431,11 +35811,6 @@
       <c r="J731" t="n">
         <v>2014</v>
       </c>
-      <c r="L731" t="inlineStr">
-        <is>
-          <t>MUNI DIST MANUEL A MESONES MURO PPT</t>
-        </is>
-      </c>
     </row>
     <row r="732">
       <c r="A732" t="inlineStr">
@@ -36477,11 +35852,6 @@
       <c r="J732" t="n">
         <v>2014</v>
       </c>
-      <c r="L732" t="inlineStr">
-        <is>
-          <t>MUNI DIST PITIPO PPTO</t>
-        </is>
-      </c>
     </row>
     <row r="733">
       <c r="A733" t="inlineStr">
@@ -36523,11 +35893,6 @@
       <c r="J733" t="n">
         <v>2014</v>
       </c>
-      <c r="L733" t="inlineStr">
-        <is>
-          <t>MUNI DIST CIUDAD ETEN PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="734">
       <c r="A734" t="inlineStr">
@@ -36569,11 +35934,6 @@
       <c r="J734" t="n">
         <v>2014</v>
       </c>
-      <c r="L734" t="inlineStr">
-        <is>
-          <t>MUNI DIST PITIPO PPTO</t>
-        </is>
-      </c>
     </row>
     <row r="735">
       <c r="A735" t="inlineStr">
@@ -36615,11 +35975,6 @@
       <c r="J735" t="n">
         <v>2014</v>
       </c>
-      <c r="L735" t="inlineStr">
-        <is>
-          <t>MUNI DIST PITIPO PPTO</t>
-        </is>
-      </c>
     </row>
     <row r="736">
       <c r="A736" t="inlineStr">
@@ -36671,9 +36026,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N736" t="n">
-        <v>7000016372</v>
-      </c>
     </row>
     <row r="737">
       <c r="A737" t="inlineStr">
@@ -36715,14 +36067,6 @@
       <c r="J737" t="n">
         <v>2014</v>
       </c>
-      <c r="L737" t="inlineStr">
-        <is>
-          <t>GERENCIA REGIONAL DE EDUCACION LAMB</t>
-        </is>
-      </c>
-      <c r="N737" t="n">
-        <v>7000016313</v>
-      </c>
     </row>
     <row r="738">
       <c r="A738" t="inlineStr">
@@ -36825,9 +36169,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N739" t="n">
-        <v>7000016567</v>
-      </c>
     </row>
     <row r="740">
       <c r="A740" t="inlineStr">
@@ -36930,9 +36271,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N741" t="n">
-        <v>7000016404</v>
-      </c>
     </row>
     <row r="742">
       <c r="A742" t="inlineStr">
@@ -36984,9 +36322,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N742" t="n">
-        <v>7000016403</v>
-      </c>
     </row>
     <row r="743">
       <c r="A743" t="inlineStr">
@@ -37038,9 +36373,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N743" t="n">
-        <v>7000016401</v>
-      </c>
     </row>
     <row r="744">
       <c r="A744" t="inlineStr">
@@ -37092,9 +36424,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N744" t="n">
-        <v>7000016400</v>
-      </c>
     </row>
     <row r="745">
       <c r="A745" t="inlineStr">
@@ -37146,9 +36475,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N745" t="n">
-        <v>7000016424</v>
-      </c>
     </row>
     <row r="746">
       <c r="A746" t="inlineStr">
@@ -37200,9 +36526,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N746" t="n">
-        <v>7000016392</v>
-      </c>
     </row>
     <row r="747">
       <c r="A747" t="inlineStr">
@@ -37254,9 +36577,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N747" t="n">
-        <v>7000016402</v>
-      </c>
     </row>
     <row r="748">
       <c r="A748" t="inlineStr">
@@ -37308,9 +36628,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N748" t="n">
-        <v>7000016427</v>
-      </c>
     </row>
     <row r="749">
       <c r="A749" t="inlineStr">
@@ -37362,9 +36679,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N749" t="n">
-        <v>7000016389</v>
-      </c>
     </row>
     <row r="750">
       <c r="A750" t="inlineStr">
@@ -37416,9 +36730,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N750" t="n">
-        <v>7000016366</v>
-      </c>
     </row>
     <row r="751">
       <c r="A751" t="inlineStr">
@@ -37470,9 +36781,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N751" t="n">
-        <v>7000016570</v>
-      </c>
     </row>
     <row r="752">
       <c r="A752" t="inlineStr">
@@ -37524,9 +36832,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N752" t="n">
-        <v>7000016393</v>
-      </c>
     </row>
     <row r="753">
       <c r="A753" t="inlineStr">
@@ -37578,9 +36883,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N753" t="n">
-        <v>7000016360</v>
-      </c>
     </row>
     <row r="754">
       <c r="A754" t="inlineStr">
@@ -37622,11 +36924,6 @@
       <c r="J754" t="n">
         <v>2014</v>
       </c>
-      <c r="L754" t="inlineStr">
-        <is>
-          <t>MINISTERIO PUBLICO-GERENCIA ADMINIS</t>
-        </is>
-      </c>
     </row>
     <row r="755">
       <c r="A755" t="inlineStr">
@@ -37729,9 +37026,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N756" t="n">
-        <v>7000016598</v>
-      </c>
     </row>
     <row r="757">
       <c r="A757" t="inlineStr">
@@ -37783,9 +37077,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N757" t="n">
-        <v>7000016354</v>
-      </c>
     </row>
     <row r="758">
       <c r="A758" t="inlineStr">
@@ -37837,9 +37128,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N758" t="n">
-        <v>7000016576</v>
-      </c>
     </row>
     <row r="759">
       <c r="A759" t="inlineStr">
@@ -37891,9 +37179,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N759" t="n">
-        <v>7000016558</v>
-      </c>
     </row>
     <row r="760">
       <c r="A760" t="inlineStr">
@@ -37945,9 +37230,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N760" t="n">
-        <v>7000016387</v>
-      </c>
     </row>
     <row r="761">
       <c r="A761" t="inlineStr">
@@ -37999,9 +37281,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N761" t="n">
-        <v>7000016422</v>
-      </c>
     </row>
     <row r="762">
       <c r="A762" t="inlineStr">
@@ -38053,9 +37332,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N762" t="n">
-        <v>7000016411</v>
-      </c>
     </row>
     <row r="763">
       <c r="A763" t="inlineStr">
@@ -38107,9 +37383,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N763" t="n">
-        <v>7000016352</v>
-      </c>
     </row>
     <row r="764">
       <c r="A764" t="inlineStr">
@@ -38161,9 +37434,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N764" t="n">
-        <v>7000016407</v>
-      </c>
     </row>
     <row r="765">
       <c r="A765" t="inlineStr">
@@ -38205,9 +37475,6 @@
       <c r="J765" t="n">
         <v>1013</v>
       </c>
-      <c r="N765" t="n">
-        <v>7000016374</v>
-      </c>
     </row>
     <row r="766">
       <c r="A766" t="inlineStr">
@@ -38259,9 +37526,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N766" t="n">
-        <v>7000016409</v>
-      </c>
     </row>
     <row r="767">
       <c r="A767" t="inlineStr">
@@ -38313,9 +37577,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N767" t="n">
-        <v>7000016391</v>
-      </c>
     </row>
     <row r="768">
       <c r="A768" t="inlineStr">
@@ -38367,9 +37628,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N768" t="n">
-        <v>7000016377</v>
-      </c>
     </row>
     <row r="769">
       <c r="A769" t="inlineStr">
@@ -38421,9 +37679,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N769" t="n">
-        <v>7000016596</v>
-      </c>
     </row>
     <row r="770">
       <c r="A770" t="inlineStr">
@@ -38475,9 +37730,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N770" t="n">
-        <v>7000016565</v>
-      </c>
     </row>
     <row r="771">
       <c r="A771" t="inlineStr">
@@ -38529,9 +37781,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N771" t="n">
-        <v>7000016355</v>
-      </c>
     </row>
     <row r="772">
       <c r="A772" t="inlineStr">
@@ -38583,9 +37832,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N772" t="n">
-        <v>7000016569</v>
-      </c>
     </row>
     <row r="773">
       <c r="A773" t="inlineStr">
@@ -38637,9 +37883,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N773" t="n">
-        <v>7000016414</v>
-      </c>
     </row>
     <row r="774">
       <c r="A774" t="inlineStr">
@@ -38691,9 +37934,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N774" t="n">
-        <v>7000016388</v>
-      </c>
     </row>
     <row r="775">
       <c r="A775" t="inlineStr">
@@ -38745,9 +37985,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N775" t="n">
-        <v>7000016412</v>
-      </c>
     </row>
     <row r="776">
       <c r="A776" t="inlineStr">
@@ -38799,9 +38036,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N776" t="n">
-        <v>7000016381</v>
-      </c>
     </row>
     <row r="777">
       <c r="A777" t="inlineStr">
@@ -38853,9 +38087,6 @@
           <t>TRABAJADOR</t>
         </is>
       </c>
-      <c r="N777" t="n">
-        <v>100057087</v>
-      </c>
     </row>
     <row r="778">
       <c r="A778" t="inlineStr">
@@ -38907,9 +38138,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N778" t="n">
-        <v>7000016559</v>
-      </c>
     </row>
     <row r="779">
       <c r="A779" t="inlineStr">
@@ -38961,9 +38189,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N779" t="n">
-        <v>7000016390</v>
-      </c>
     </row>
     <row r="780">
       <c r="A780" t="inlineStr">
@@ -39015,9 +38240,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N780" t="n">
-        <v>7000016600</v>
-      </c>
     </row>
     <row r="781">
       <c r="A781" t="inlineStr">
@@ -39069,9 +38291,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N781" t="n">
-        <v>7000016368</v>
-      </c>
     </row>
     <row r="782">
       <c r="A782" t="inlineStr">
@@ -39123,9 +38342,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N782" t="n">
-        <v>7000016376</v>
-      </c>
     </row>
     <row r="783">
       <c r="A783" t="inlineStr">
@@ -39177,9 +38393,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N783" t="n">
-        <v>7000016351</v>
-      </c>
     </row>
     <row r="784">
       <c r="A784" t="inlineStr">
@@ -39282,9 +38495,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N785" t="n">
-        <v>7000016413</v>
-      </c>
     </row>
     <row r="786">
       <c r="A786" t="inlineStr">
@@ -39387,9 +38597,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N787" t="n">
-        <v>7000016410</v>
-      </c>
     </row>
     <row r="788">
       <c r="A788" t="inlineStr">
@@ -39441,9 +38648,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N788" t="n">
-        <v>7000016397</v>
-      </c>
     </row>
     <row r="789">
       <c r="A789" t="inlineStr">
@@ -39495,9 +38699,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N789" t="n">
-        <v>7000016384</v>
-      </c>
     </row>
     <row r="790">
       <c r="A790" t="inlineStr">
@@ -39549,9 +38750,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N790" t="n">
-        <v>7000016553</v>
-      </c>
     </row>
     <row r="791">
       <c r="A791" t="inlineStr">
@@ -39705,9 +38903,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N793" t="n">
-        <v>7000016566</v>
-      </c>
     </row>
     <row r="794">
       <c r="A794" t="inlineStr">
@@ -39810,9 +39005,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N795" t="n">
-        <v>7000016394</v>
-      </c>
     </row>
     <row r="796">
       <c r="A796" t="inlineStr">
@@ -39864,9 +39056,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N796" t="n">
-        <v>7000016353</v>
-      </c>
     </row>
     <row r="797">
       <c r="A797" t="inlineStr">
@@ -39918,9 +39107,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N797" t="n">
-        <v>7000016555</v>
-      </c>
     </row>
     <row r="798">
       <c r="A798" t="inlineStr">
@@ -40023,9 +39209,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N799" t="n">
-        <v>7000016379</v>
-      </c>
     </row>
     <row r="800">
       <c r="A800" t="inlineStr">
@@ -40077,9 +39260,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N800" t="n">
-        <v>7000016428</v>
-      </c>
     </row>
     <row r="801">
       <c r="A801" t="inlineStr">
@@ -40172,11 +39352,6 @@
       <c r="J802" t="n">
         <v>2014</v>
       </c>
-      <c r="L802" t="inlineStr">
-        <is>
-          <t>GOB LAMBAY-HOSP DOC LAS MERCED PPTO</t>
-        </is>
-      </c>
     </row>
     <row r="803">
       <c r="A803" t="inlineStr">
@@ -40279,9 +39454,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N804" t="n">
-        <v>7000016408</v>
-      </c>
     </row>
     <row r="805">
       <c r="A805" t="inlineStr">
@@ -40333,9 +39505,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N805" t="n">
-        <v>7000016416</v>
-      </c>
     </row>
     <row r="806">
       <c r="A806" t="inlineStr">
@@ -40438,9 +39607,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N807" t="n">
-        <v>7000016364</v>
-      </c>
     </row>
     <row r="808">
       <c r="A808" t="inlineStr">
@@ -40492,9 +39658,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N808" t="n">
-        <v>7000016568</v>
-      </c>
     </row>
     <row r="809">
       <c r="A809" t="inlineStr">
@@ -40546,9 +39709,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N809" t="n">
-        <v>7000016554</v>
-      </c>
     </row>
     <row r="810">
       <c r="A810" t="inlineStr">
@@ -40600,9 +39760,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N810" t="n">
-        <v>7000016358</v>
-      </c>
     </row>
     <row r="811">
       <c r="A811" t="inlineStr">
@@ -40654,9 +39811,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N811" t="n">
-        <v>7000016426</v>
-      </c>
     </row>
     <row r="812">
       <c r="A812" t="inlineStr">
@@ -40708,9 +39862,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N812" t="n">
-        <v>7000016425</v>
-      </c>
     </row>
     <row r="813">
       <c r="A813" t="inlineStr">
@@ -40762,9 +39913,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N813" t="n">
-        <v>7000016423</v>
-      </c>
     </row>
     <row r="814">
       <c r="A814" t="inlineStr">
@@ -40816,9 +39964,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N814" t="n">
-        <v>7000016370</v>
-      </c>
     </row>
     <row r="815">
       <c r="A815" t="inlineStr">
@@ -40870,9 +40015,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N815" t="n">
-        <v>7000016398</v>
-      </c>
     </row>
     <row r="816">
       <c r="A816" t="inlineStr">
@@ -41026,9 +40168,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N818" t="n">
-        <v>7000016369</v>
-      </c>
     </row>
     <row r="819">
       <c r="A819" t="inlineStr">
@@ -41182,9 +40321,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N821" t="n">
-        <v>7000016365</v>
-      </c>
     </row>
     <row r="822">
       <c r="A822" t="inlineStr">
@@ -41236,9 +40372,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N822" t="n">
-        <v>7000016363</v>
-      </c>
     </row>
     <row r="823">
       <c r="A823" t="inlineStr">
@@ -41290,9 +40423,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N823" t="n">
-        <v>7000016362</v>
-      </c>
     </row>
     <row r="824">
       <c r="A824" t="inlineStr">
@@ -41344,9 +40474,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N824" t="n">
-        <v>7000016417</v>
-      </c>
     </row>
     <row r="825">
       <c r="A825" t="inlineStr">
@@ -41398,9 +40525,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N825" t="n">
-        <v>7000016415</v>
-      </c>
     </row>
     <row r="826">
       <c r="A826" t="inlineStr">
@@ -41452,9 +40576,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N826" t="n">
-        <v>7000016385</v>
-      </c>
     </row>
     <row r="827">
       <c r="A827" t="inlineStr">
@@ -41506,9 +40627,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N827" t="n">
-        <v>7000016421</v>
-      </c>
     </row>
     <row r="828">
       <c r="A828" t="inlineStr">
@@ -41560,9 +40678,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N828" t="n">
-        <v>7000016396</v>
-      </c>
     </row>
     <row r="829">
       <c r="A829" t="inlineStr">
@@ -41614,9 +40729,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N829" t="n">
-        <v>7000016420</v>
-      </c>
     </row>
     <row r="830">
       <c r="A830" t="inlineStr">
@@ -41668,9 +40780,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N830" t="n">
-        <v>7000016406</v>
-      </c>
     </row>
     <row r="831">
       <c r="A831" t="inlineStr">
@@ -41773,9 +40882,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N832" t="n">
-        <v>7000016367</v>
-      </c>
     </row>
     <row r="833">
       <c r="A833" t="inlineStr">
@@ -41827,9 +40933,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N833" t="n">
-        <v>7000016375</v>
-      </c>
     </row>
     <row r="834">
       <c r="A834" t="inlineStr">
@@ -41881,9 +40984,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N834" t="n">
-        <v>7000016380</v>
-      </c>
     </row>
     <row r="835">
       <c r="A835" t="inlineStr">
@@ -41986,9 +41086,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N836" t="n">
-        <v>7000016361</v>
-      </c>
     </row>
     <row r="837">
       <c r="A837" t="inlineStr">
@@ -42040,9 +41137,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N837" t="n">
-        <v>7000016395</v>
-      </c>
     </row>
     <row r="838">
       <c r="A838" t="inlineStr">
@@ -42084,11 +41178,6 @@
       <c r="J838" t="n">
         <v>2014</v>
       </c>
-      <c r="L838" t="inlineStr">
-        <is>
-          <t>II DIR TERRITORIAL POLICIA CHICLAYO</t>
-        </is>
-      </c>
     </row>
     <row r="839">
       <c r="A839" t="inlineStr">
@@ -42140,9 +41229,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N839" t="n">
-        <v>7000016419</v>
-      </c>
     </row>
     <row r="840">
       <c r="A840" t="inlineStr">
@@ -42194,9 +41280,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N840" t="n">
-        <v>7000016356</v>
-      </c>
     </row>
     <row r="841">
       <c r="A841" t="inlineStr">
@@ -42248,9 +41331,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N841" t="n">
-        <v>7000016383</v>
-      </c>
     </row>
     <row r="842">
       <c r="A842" t="inlineStr">
@@ -42302,9 +41382,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N842" t="n">
-        <v>7000016359</v>
-      </c>
     </row>
     <row r="843">
       <c r="A843" t="inlineStr">
@@ -42356,9 +41433,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N843" t="n">
-        <v>7000016382</v>
-      </c>
     </row>
     <row r="844">
       <c r="A844" t="inlineStr">
@@ -42461,9 +41535,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N845" t="n">
-        <v>7000016357</v>
-      </c>
     </row>
     <row r="846">
       <c r="A846" t="inlineStr">
@@ -42515,9 +41586,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N846" t="n">
-        <v>7000016405</v>
-      </c>
     </row>
     <row r="847">
       <c r="A847" t="inlineStr">
@@ -42569,9 +41637,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N847" t="n">
-        <v>7000016386</v>
-      </c>
     </row>
     <row r="848">
       <c r="A848" t="inlineStr">
@@ -42623,9 +41688,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N848" t="n">
-        <v>7000016378</v>
-      </c>
     </row>
     <row r="849">
       <c r="A849" t="inlineStr">
@@ -42677,9 +41739,6 @@
           <t>TRABAJADOR</t>
         </is>
       </c>
-      <c r="N849" t="n">
-        <v>100056246</v>
-      </c>
     </row>
     <row r="850">
       <c r="A850" t="inlineStr">
@@ -42731,9 +41790,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N850" t="n">
-        <v>7000016399</v>
-      </c>
     </row>
     <row r="851">
       <c r="A851" t="inlineStr">
@@ -42887,9 +41943,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N853" t="n">
-        <v>7000016599</v>
-      </c>
     </row>
     <row r="854">
       <c r="A854" t="inlineStr">
@@ -42941,9 +41994,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N854" t="n">
-        <v>7000016597</v>
-      </c>
     </row>
     <row r="855">
       <c r="A855" t="inlineStr">
@@ -42995,9 +42045,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N855" t="n">
-        <v>7000016373</v>
-      </c>
     </row>
     <row r="856">
       <c r="A856" t="inlineStr">
@@ -43049,9 +42096,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N856" t="n">
-        <v>7000016453</v>
-      </c>
     </row>
     <row r="857">
       <c r="A857" t="inlineStr">
@@ -43098,14 +42142,6 @@
           <t>01 0F061 0013976</t>
         </is>
       </c>
-      <c r="L857" t="inlineStr">
-        <is>
-          <t>STATKRAFT PERU S.A.</t>
-        </is>
-      </c>
-      <c r="N857" t="n">
-        <v>6500005047</v>
-      </c>
     </row>
     <row r="858">
       <c r="A858" t="inlineStr">
@@ -43924,9 +42960,6 @@
       <c r="J875" t="n">
         <v>2505</v>
       </c>
-      <c r="N875" t="n">
-        <v>100032981</v>
-      </c>
     </row>
     <row r="876">
       <c r="A876" t="inlineStr">
@@ -43968,9 +43001,6 @@
       <c r="J876" t="n">
         <v>2505</v>
       </c>
-      <c r="N876" t="n">
-        <v>100032573</v>
-      </c>
     </row>
     <row r="877">
       <c r="A877" t="inlineStr">
@@ -44012,8 +43042,10 @@
       <c r="J877" t="n">
         <v>2406</v>
       </c>
-      <c r="N877" t="n">
-        <v>100032572</v>
+      <c r="L877" t="inlineStr">
+        <is>
+          <t>EMPRESA REGIONAL DE SERVICIO PUBLICO DE ELECTRICIDAD DEL NORTE S.A.</t>
+        </is>
       </c>
     </row>
     <row r="878">
@@ -44056,9 +43088,6 @@
       <c r="J878" t="n">
         <v>2505</v>
       </c>
-      <c r="N878" t="n">
-        <v>100032571</v>
-      </c>
     </row>
     <row r="879">
       <c r="A879" t="inlineStr">
@@ -44100,8 +43129,10 @@
       <c r="J879" t="n">
         <v>2406</v>
       </c>
-      <c r="N879" t="n">
-        <v>100032570</v>
+      <c r="L879" t="inlineStr">
+        <is>
+          <t>EMPRESA REGIONAL DE SERVICIO PUBLICO DE ELECTRICIDAD DEL NORTE S.A.</t>
+        </is>
       </c>
     </row>
     <row r="880">
@@ -44154,9 +43185,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N880" t="n">
-        <v>7000016311</v>
-      </c>
     </row>
     <row r="881">
       <c r="A881" t="inlineStr">
@@ -44203,11 +43231,6 @@
           <t>Referencia Beneficiari</t>
         </is>
       </c>
-      <c r="L881" t="inlineStr">
-        <is>
-          <t>WESTERN UNION PERU S.A.</t>
-        </is>
-      </c>
     </row>
     <row r="882">
       <c r="A882" t="inlineStr">
@@ -44249,11 +43272,6 @@
       <c r="J882" t="n">
         <v>2014</v>
       </c>
-      <c r="L882" t="inlineStr">
-        <is>
-          <t>MUNI DIST MOCHUMI PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="883">
       <c r="A883" t="inlineStr">
@@ -44295,11 +43313,6 @@
       <c r="J883" t="n">
         <v>2014</v>
       </c>
-      <c r="L883" t="inlineStr">
-        <is>
-          <t>MUNI DIST REQUE PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="884">
       <c r="A884" t="inlineStr">
@@ -44341,8 +43354,10 @@
       <c r="J884" t="n">
         <v>2401</v>
       </c>
-      <c r="N884" t="n">
-        <v>7000016026</v>
+      <c r="L884" t="inlineStr">
+        <is>
+          <t>CAJA MUNICIPAL DE AHORRO Y CREDITO DE AREQUIPA</t>
+        </is>
       </c>
     </row>
     <row r="885">
@@ -44385,6 +43400,11 @@
       <c r="J885" t="n">
         <v>2401</v>
       </c>
+      <c r="L885" t="inlineStr">
+        <is>
+          <t>CONSORCIO ELECTRICO DE VILLACURI S.A.C.</t>
+        </is>
+      </c>
     </row>
     <row r="886">
       <c r="A886" t="inlineStr">
@@ -44426,11 +43446,6 @@
       <c r="J886" t="n">
         <v>2014</v>
       </c>
-      <c r="L886" t="inlineStr">
-        <is>
-          <t>MUNI DIST SAN JOSE PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="887">
       <c r="A887" t="inlineStr">
@@ -44482,9 +43497,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N887" t="n">
-        <v>7000016309</v>
-      </c>
     </row>
     <row r="888">
       <c r="A888" t="inlineStr">
@@ -44526,11 +43538,6 @@
       <c r="J888" t="n">
         <v>2014</v>
       </c>
-      <c r="L888" t="inlineStr">
-        <is>
-          <t>MUNI DIST SAN JOSE PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="889">
       <c r="A889" t="inlineStr">
@@ -44582,9 +43589,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N889" t="n">
-        <v>7000016237</v>
-      </c>
     </row>
     <row r="890">
       <c r="A890" t="inlineStr">
@@ -44636,9 +43640,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N890" t="n">
-        <v>7000016595</v>
-      </c>
     </row>
     <row r="891">
       <c r="A891" t="inlineStr">
@@ -44690,9 +43691,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N891" t="n">
-        <v>7000016199</v>
-      </c>
     </row>
     <row r="892">
       <c r="A892" t="inlineStr">
@@ -44744,9 +43742,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N892" t="n">
-        <v>7000016543</v>
-      </c>
     </row>
     <row r="893">
       <c r="A893" t="inlineStr">
@@ -44798,9 +43793,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N893" t="n">
-        <v>7000016548</v>
-      </c>
     </row>
     <row r="894">
       <c r="A894" t="inlineStr">
@@ -44852,9 +43844,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N894" t="n">
-        <v>7000016255</v>
-      </c>
     </row>
     <row r="895">
       <c r="A895" t="inlineStr">
@@ -44957,9 +43946,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N896" t="n">
-        <v>7000016258</v>
-      </c>
     </row>
     <row r="897">
       <c r="A897" t="inlineStr">
@@ -45011,9 +43997,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N897" t="n">
-        <v>7000016564</v>
-      </c>
     </row>
     <row r="898">
       <c r="A898" t="inlineStr">
@@ -45065,9 +44048,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N898" t="n">
-        <v>7000016542</v>
-      </c>
     </row>
     <row r="899">
       <c r="A899" t="inlineStr">
@@ -45119,9 +44099,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N899" t="n">
-        <v>7000016225</v>
-      </c>
     </row>
     <row r="900">
       <c r="A900" t="inlineStr">
@@ -45173,9 +44150,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N900" t="n">
-        <v>7000016202</v>
-      </c>
     </row>
     <row r="901">
       <c r="A901" t="inlineStr">
@@ -45227,9 +44201,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N901" t="n">
-        <v>7000016539</v>
-      </c>
     </row>
     <row r="902">
       <c r="A902" t="inlineStr">
@@ -45281,9 +44252,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N902" t="n">
-        <v>7000016547</v>
-      </c>
     </row>
     <row r="903">
       <c r="A903" t="inlineStr">
@@ -45325,11 +44293,6 @@
       <c r="J903" t="n">
         <v>2014</v>
       </c>
-      <c r="L903" t="inlineStr">
-        <is>
-          <t>SENASA PPTO 2003</t>
-        </is>
-      </c>
     </row>
     <row r="904">
       <c r="A904" t="inlineStr">
@@ -45381,9 +44344,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N904" t="n">
-        <v>7000016214</v>
-      </c>
     </row>
     <row r="905">
       <c r="A905" t="inlineStr">
@@ -45425,11 +44385,6 @@
       <c r="J905" t="n">
         <v>2014</v>
       </c>
-      <c r="L905" t="inlineStr">
-        <is>
-          <t>MUNI DIST PUERTO ETEN PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="906">
       <c r="A906" t="inlineStr">
@@ -45481,9 +44436,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N906" t="n">
-        <v>7000016557</v>
-      </c>
     </row>
     <row r="907">
       <c r="A907" t="inlineStr">
@@ -45535,9 +44487,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N907" t="n">
-        <v>7000016207</v>
-      </c>
     </row>
     <row r="908">
       <c r="A908" t="inlineStr">
@@ -45589,9 +44538,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N908" t="n">
-        <v>7000016206</v>
-      </c>
     </row>
     <row r="909">
       <c r="A909" t="inlineStr">
@@ -45643,9 +44589,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N909" t="n">
-        <v>7000016245</v>
-      </c>
     </row>
     <row r="910">
       <c r="A910" t="inlineStr">
@@ -45697,9 +44640,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N910" t="n">
-        <v>7000016526</v>
-      </c>
     </row>
     <row r="911">
       <c r="A911" t="inlineStr">
@@ -45751,9 +44691,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N911" t="n">
-        <v>7000016222</v>
-      </c>
     </row>
     <row r="912">
       <c r="A912" t="inlineStr">
@@ -45805,9 +44742,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N912" t="n">
-        <v>7000016243</v>
-      </c>
     </row>
     <row r="913">
       <c r="A913" t="inlineStr">
@@ -45859,9 +44793,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N913" t="n">
-        <v>7000016528</v>
-      </c>
     </row>
     <row r="914">
       <c r="A914" t="inlineStr">
@@ -45913,9 +44844,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N914" t="n">
-        <v>7000016201</v>
-      </c>
     </row>
     <row r="915">
       <c r="A915" t="inlineStr">
@@ -45967,9 +44895,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N915" t="n">
-        <v>7000016249</v>
-      </c>
     </row>
     <row r="916">
       <c r="A916" t="inlineStr">
@@ -46072,9 +44997,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N917" t="n">
-        <v>7000016241</v>
-      </c>
     </row>
     <row r="918">
       <c r="A918" t="inlineStr">
@@ -46126,9 +45048,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N918" t="n">
-        <v>7000016240</v>
-      </c>
     </row>
     <row r="919">
       <c r="A919" t="inlineStr">
@@ -46180,9 +45099,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N919" t="n">
-        <v>7000016239</v>
-      </c>
     </row>
     <row r="920">
       <c r="A920" t="inlineStr">
@@ -46234,9 +45150,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N920" t="n">
-        <v>7000016527</v>
-      </c>
     </row>
     <row r="921">
       <c r="A921" t="inlineStr">
@@ -46288,9 +45201,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N921" t="n">
-        <v>7000016611</v>
-      </c>
     </row>
     <row r="922">
       <c r="A922" t="inlineStr">
@@ -46342,9 +45252,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N922" t="n">
-        <v>7000016210</v>
-      </c>
     </row>
     <row r="923">
       <c r="A923" t="inlineStr">
@@ -46396,9 +45303,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N923" t="n">
-        <v>7000016223</v>
-      </c>
     </row>
     <row r="924">
       <c r="A924" t="inlineStr">
@@ -46450,9 +45354,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N924" t="n">
-        <v>7000016238</v>
-      </c>
     </row>
     <row r="925">
       <c r="A925" t="inlineStr">
@@ -46504,9 +45405,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N925" t="n">
-        <v>7000016532</v>
-      </c>
     </row>
     <row r="926">
       <c r="A926" t="inlineStr">
@@ -46558,9 +45456,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N926" t="n">
-        <v>7000016545</v>
-      </c>
     </row>
     <row r="927">
       <c r="A927" t="inlineStr">
@@ -46612,9 +45507,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N927" t="n">
-        <v>7000016246</v>
-      </c>
     </row>
     <row r="928">
       <c r="A928" t="inlineStr">
@@ -46666,9 +45558,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N928" t="n">
-        <v>7000016221</v>
-      </c>
     </row>
     <row r="929">
       <c r="A929" t="inlineStr">
@@ -46720,9 +45609,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N929" t="n">
-        <v>7000016680</v>
-      </c>
     </row>
     <row r="930">
       <c r="A930" t="inlineStr">
@@ -46774,9 +45660,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N930" t="n">
-        <v>7000016253</v>
-      </c>
     </row>
     <row r="931">
       <c r="A931" t="inlineStr">
@@ -46828,9 +45711,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N931" t="n">
-        <v>7000016203</v>
-      </c>
     </row>
     <row r="932">
       <c r="A932" t="inlineStr">
@@ -46882,9 +45762,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N932" t="n">
-        <v>7000016248</v>
-      </c>
     </row>
     <row r="933">
       <c r="A933" t="inlineStr">
@@ -46987,9 +45864,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N934" t="n">
-        <v>7000016529</v>
-      </c>
     </row>
     <row r="935">
       <c r="A935" t="inlineStr">
@@ -47031,11 +45905,6 @@
       <c r="J935" t="n">
         <v>2014</v>
       </c>
-      <c r="L935" t="inlineStr">
-        <is>
-          <t>SENASA PPTO 2003</t>
-        </is>
-      </c>
     </row>
     <row r="936">
       <c r="A936" t="inlineStr">
@@ -47087,9 +45956,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N936" t="n">
-        <v>7000016537</v>
-      </c>
     </row>
     <row r="937">
       <c r="A937" t="inlineStr">
@@ -47141,9 +46007,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N937" t="n">
-        <v>7000016251</v>
-      </c>
     </row>
     <row r="938">
       <c r="A938" t="inlineStr">
@@ -47185,11 +46048,6 @@
       <c r="J938" t="n">
         <v>2014</v>
       </c>
-      <c r="L938" t="inlineStr">
-        <is>
-          <t>MUNI DIST MOCHUMI PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="939">
       <c r="A939" t="inlineStr">
@@ -47231,11 +46089,6 @@
       <c r="J939" t="n">
         <v>2014</v>
       </c>
-      <c r="L939" t="inlineStr">
-        <is>
-          <t>MUNI DIST MOCHUMI PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="940">
       <c r="A940" t="inlineStr">
@@ -47277,11 +46130,6 @@
       <c r="J940" t="n">
         <v>2014</v>
       </c>
-      <c r="L940" t="inlineStr">
-        <is>
-          <t>MUNI DIST MOCHUMI PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="941">
       <c r="A941" t="inlineStr">
@@ -47323,11 +46171,6 @@
       <c r="J941" t="n">
         <v>2014</v>
       </c>
-      <c r="L941" t="inlineStr">
-        <is>
-          <t>MUNI DIST MOCHUMI PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="942">
       <c r="A942" t="inlineStr">
@@ -47379,9 +46222,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N942" t="n">
-        <v>7000016538</v>
-      </c>
     </row>
     <row r="943">
       <c r="A943" t="inlineStr">
@@ -47433,9 +46273,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N943" t="n">
-        <v>7000016536</v>
-      </c>
     </row>
     <row r="944">
       <c r="A944" t="inlineStr">
@@ -47487,9 +46324,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N944" t="n">
-        <v>7000016531</v>
-      </c>
     </row>
     <row r="945">
       <c r="A945" t="inlineStr">
@@ -47541,9 +46375,6 @@
           <t>TRABAJADOR</t>
         </is>
       </c>
-      <c r="N945" t="n">
-        <v>100057088</v>
-      </c>
     </row>
     <row r="946">
       <c r="A946" t="inlineStr">
@@ -47595,9 +46426,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N946" t="n">
-        <v>7000016310</v>
-      </c>
     </row>
     <row r="947">
       <c r="A947" t="inlineStr">
@@ -47649,9 +46477,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N947" t="n">
-        <v>7000016224</v>
-      </c>
     </row>
     <row r="948">
       <c r="A948" t="inlineStr">
@@ -47703,9 +46528,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N948" t="n">
-        <v>7000016312</v>
-      </c>
     </row>
     <row r="949">
       <c r="A949" t="inlineStr">
@@ -47747,11 +46569,6 @@
       <c r="J949" t="n">
         <v>2014</v>
       </c>
-      <c r="L949" t="inlineStr">
-        <is>
-          <t>MUNI DIST MOCHUMI PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="950">
       <c r="A950" t="inlineStr">
@@ -47803,9 +46620,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N950" t="n">
-        <v>7000016541</v>
-      </c>
     </row>
     <row r="951">
       <c r="A951" t="inlineStr">
@@ -47847,11 +46661,6 @@
       <c r="J951" t="n">
         <v>2014</v>
       </c>
-      <c r="L951" t="inlineStr">
-        <is>
-          <t>MUNI DIST SAN JOSE PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="952">
       <c r="A952" t="inlineStr">
@@ -47893,11 +46702,6 @@
       <c r="J952" t="n">
         <v>2014</v>
       </c>
-      <c r="L952" t="inlineStr">
-        <is>
-          <t>MUNI DIST SAN JOSE PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="953">
       <c r="A953" t="inlineStr">
@@ -47949,9 +46753,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N953" t="n">
-        <v>7000016257</v>
-      </c>
     </row>
     <row r="954">
       <c r="A954" t="inlineStr">
@@ -48003,9 +46804,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N954" t="n">
-        <v>7000016256</v>
-      </c>
     </row>
     <row r="955">
       <c r="A955" t="inlineStr">
@@ -48057,9 +46855,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N955" t="n">
-        <v>7000016250</v>
-      </c>
     </row>
     <row r="956">
       <c r="A956" t="inlineStr">
@@ -48111,9 +46906,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N956" t="n">
-        <v>7000016610</v>
-      </c>
     </row>
     <row r="957">
       <c r="A957" t="inlineStr">
@@ -48165,9 +46957,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N957" t="n">
-        <v>7000016226</v>
-      </c>
     </row>
     <row r="958">
       <c r="A958" t="inlineStr">
@@ -48270,9 +47059,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N959" t="n">
-        <v>7000016212</v>
-      </c>
     </row>
     <row r="960">
       <c r="A960" t="inlineStr">
@@ -48324,9 +47110,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N960" t="n">
-        <v>7000016350</v>
-      </c>
     </row>
     <row r="961">
       <c r="A961" t="inlineStr">
@@ -48419,11 +47202,6 @@
       <c r="J962" t="n">
         <v>2014</v>
       </c>
-      <c r="L962" t="inlineStr">
-        <is>
-          <t>MUNI DIST SAN JOSE PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="963">
       <c r="A963" t="inlineStr">
@@ -48526,9 +47304,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N964" t="n">
-        <v>7000016544</v>
-      </c>
     </row>
     <row r="965">
       <c r="A965" t="inlineStr">
@@ -48580,9 +47355,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N965" t="n">
-        <v>7000016219</v>
-      </c>
     </row>
     <row r="966">
       <c r="A966" t="inlineStr">
@@ -48634,9 +47406,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N966" t="n">
-        <v>7000016252</v>
-      </c>
     </row>
     <row r="967">
       <c r="A967" t="inlineStr">
@@ -48688,9 +47457,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N967" t="n">
-        <v>7000016549</v>
-      </c>
     </row>
     <row r="968">
       <c r="A968" t="inlineStr">
@@ -48742,9 +47508,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N968" t="n">
-        <v>7000016540</v>
-      </c>
     </row>
     <row r="969">
       <c r="A969" t="inlineStr">
@@ -48796,9 +47559,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N969" t="n">
-        <v>7000016254</v>
-      </c>
     </row>
     <row r="970">
       <c r="A970" t="inlineStr">
@@ -48850,9 +47610,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N970" t="n">
-        <v>7000016230</v>
-      </c>
     </row>
     <row r="971">
       <c r="A971" t="inlineStr">
@@ -48904,9 +47661,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N971" t="n">
-        <v>7000016218</v>
-      </c>
     </row>
     <row r="972">
       <c r="A972" t="inlineStr">
@@ -49009,9 +47763,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N973" t="n">
-        <v>7000016209</v>
-      </c>
     </row>
     <row r="974">
       <c r="A974" t="inlineStr">
@@ -49063,9 +47814,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N974" t="n">
-        <v>7000016205</v>
-      </c>
     </row>
     <row r="975">
       <c r="A975" t="inlineStr">
@@ -49117,9 +47865,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N975" t="n">
-        <v>7000016200</v>
-      </c>
     </row>
     <row r="976">
       <c r="A976" t="inlineStr">
@@ -49171,9 +47916,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N976" t="n">
-        <v>7000016211</v>
-      </c>
     </row>
     <row r="977">
       <c r="A977" t="inlineStr">
@@ -49225,9 +47967,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N977" t="n">
-        <v>7000016216</v>
-      </c>
     </row>
     <row r="978">
       <c r="A978" t="inlineStr">
@@ -49279,9 +48018,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N978" t="n">
-        <v>7000016242</v>
-      </c>
     </row>
     <row r="979">
       <c r="A979" t="inlineStr">
@@ -49333,9 +48069,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N979" t="n">
-        <v>7000016229</v>
-      </c>
     </row>
     <row r="980">
       <c r="A980" t="inlineStr">
@@ -49387,9 +48120,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N980" t="n">
-        <v>7000016228</v>
-      </c>
     </row>
     <row r="981">
       <c r="A981" t="inlineStr">
@@ -49441,9 +48171,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N981" t="n">
-        <v>7000016534</v>
-      </c>
     </row>
     <row r="982">
       <c r="A982" t="inlineStr">
@@ -49495,9 +48222,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N982" t="n">
-        <v>7000016247</v>
-      </c>
     </row>
     <row r="983">
       <c r="A983" t="inlineStr">
@@ -49549,9 +48273,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N983" t="n">
-        <v>7000016217</v>
-      </c>
     </row>
     <row r="984">
       <c r="A984" t="inlineStr">
@@ -49603,9 +48324,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N984" t="n">
-        <v>7000016535</v>
-      </c>
     </row>
     <row r="985">
       <c r="A985" t="inlineStr">
@@ -49657,9 +48375,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N985" t="n">
-        <v>7000016204</v>
-      </c>
     </row>
     <row r="986">
       <c r="A986" t="inlineStr">
@@ -49711,9 +48426,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N986" t="n">
-        <v>7000016235</v>
-      </c>
     </row>
     <row r="987">
       <c r="A987" t="inlineStr">
@@ -49765,9 +48477,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N987" t="n">
-        <v>7000016233</v>
-      </c>
     </row>
     <row r="988">
       <c r="A988" t="inlineStr">
@@ -49819,9 +48528,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N988" t="n">
-        <v>7000016208</v>
-      </c>
     </row>
     <row r="989">
       <c r="A989" t="inlineStr">
@@ -49873,9 +48579,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N989" t="n">
-        <v>7000016244</v>
-      </c>
     </row>
     <row r="990">
       <c r="A990" t="inlineStr">
@@ -49927,9 +48630,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N990" t="n">
-        <v>7000016236</v>
-      </c>
     </row>
     <row r="991">
       <c r="A991" t="inlineStr">
@@ -49981,9 +48681,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N991" t="n">
-        <v>7000016234</v>
-      </c>
     </row>
     <row r="992">
       <c r="A992" t="inlineStr">
@@ -50035,9 +48732,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N992" t="n">
-        <v>7000016231</v>
-      </c>
     </row>
     <row r="993">
       <c r="A993" t="inlineStr">
@@ -50089,9 +48783,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N993" t="n">
-        <v>7000016220</v>
-      </c>
     </row>
     <row r="994">
       <c r="A994" t="inlineStr">
@@ -50143,9 +48834,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N994" t="n">
-        <v>7000016215</v>
-      </c>
     </row>
     <row r="995">
       <c r="A995" t="inlineStr">
@@ -50187,11 +48875,6 @@
       <c r="J995" t="n">
         <v>2014</v>
       </c>
-      <c r="L995" t="inlineStr">
-        <is>
-          <t>MUNI DIST SAN JOSE PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="996">
       <c r="A996" t="inlineStr">
@@ -50233,11 +48916,6 @@
       <c r="J996" t="n">
         <v>2014</v>
       </c>
-      <c r="L996" t="inlineStr">
-        <is>
-          <t>MUNI DIST SAN JOSE PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="997">
       <c r="A997" t="inlineStr">
@@ -50279,11 +48957,6 @@
       <c r="J997" t="n">
         <v>2014</v>
       </c>
-      <c r="L997" t="inlineStr">
-        <is>
-          <t>MUNI DIST PUERTO ETEN PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="998">
       <c r="A998" t="inlineStr">
@@ -50335,9 +49008,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N998" t="n">
-        <v>7000016452</v>
-      </c>
     </row>
     <row r="999">
       <c r="A999" t="inlineStr">
@@ -50389,9 +49059,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N999" t="n">
-        <v>7000016451</v>
-      </c>
     </row>
     <row r="1000">
       <c r="A1000" t="inlineStr">
@@ -50494,9 +49161,6 @@
           <t>PREPAGO</t>
         </is>
       </c>
-      <c r="N1001" t="n">
-        <v>7000016227</v>
-      </c>
     </row>
     <row r="1002">
       <c r="A1002" t="inlineStr">
@@ -50548,9 +49212,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N1002" t="n">
-        <v>7000016213</v>
-      </c>
     </row>
     <row r="1003">
       <c r="A1003" t="inlineStr">
@@ -50602,9 +49263,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N1003" t="n">
-        <v>7000016232</v>
-      </c>
     </row>
     <row r="1004">
       <c r="A1004" t="inlineStr">
@@ -50646,11 +49304,6 @@
       <c r="J1004" t="n">
         <v>2014</v>
       </c>
-      <c r="L1004" t="inlineStr">
-        <is>
-          <t>MUNI DIST SAN JOSE PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="1005">
       <c r="A1005" t="inlineStr">
@@ -50692,11 +49345,6 @@
       <c r="J1005" t="n">
         <v>2014</v>
       </c>
-      <c r="L1005" t="inlineStr">
-        <is>
-          <t>MUNI DIST SAN JOSE PRESUPUESTO</t>
-        </is>
-      </c>
     </row>
     <row r="1006">
       <c r="A1006" t="inlineStr">
@@ -50748,9 +49396,6 @@
           <t>COD.RECAUDO</t>
         </is>
       </c>
-      <c r="N1006" t="n">
-        <v>7000016533</v>
-      </c>
     </row>
     <row r="1007">
       <c r="A1007" t="inlineStr">
@@ -50848,14 +49493,6 @@
           <t>PAGO DE PROVEEDORES</t>
         </is>
       </c>
-      <c r="L1008" t="inlineStr">
-        <is>
-          <t>FIDEICOMISO ELECTROPERU</t>
-        </is>
-      </c>
-      <c r="N1008" t="n">
-        <v>6500005045</v>
-      </c>
     </row>
     <row r="1009">
       <c r="A1009" t="inlineStr">
@@ -50901,14 +49538,6 @@
         <is>
           <t>Pago Fact.14007</t>
         </is>
-      </c>
-      <c r="L1009" t="inlineStr">
-        <is>
-          <t>CELEPSA RENOVABLES SRL</t>
-        </is>
-      </c>
-      <c r="N1009" t="n">
-        <v>6500005046</v>
       </c>
     </row>
   </sheetData>

</xml_diff>